<commit_message>
Dia pre-cierre de planilla
</commit_message>
<xml_diff>
--- a/1-CONTROL/2-TAREO/TAREO-MAYO.xlsx
+++ b/1-CONTROL/2-TAREO/TAREO-MAYO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AKM\1-CONTROL\2-TAREO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83434F9C-9BCC-4A80-99E5-FD2BA838EE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA49B9BA-C08E-4DC0-B8DA-EAED30191966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{100E3196-77E0-4FB0-BD0A-F462B801CA56}"/>
   </bookViews>
@@ -2463,6 +2463,24 @@
     <xf numFmtId="49" fontId="3" fillId="15" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2543,24 +2561,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3817,8 +3817,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:FK155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G156" sqref="G156"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="DE1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="EB158" sqref="EB158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3897,25 +3897,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:167" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="88"/>
+      <c r="A1" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
       <c r="V1" s="2"/>
       <c r="AA1" s="2"/>
       <c r="AF1" s="2"/>
@@ -4100,36 +4100,36 @@
       <c r="FK2" s="2"/>
     </row>
     <row r="3" spans="1:167" s="6" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="91"/>
+      <c r="A3" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="97"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="95" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y3" s="95"/>
-      <c r="Z3" s="96"/>
+      <c r="X3" s="101" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="102"/>
       <c r="AA3" s="5">
         <v>30</v>
       </c>
@@ -4298,11 +4298,11 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="95" t="s">
+      <c r="X4" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="Y4" s="95"/>
-      <c r="Z4" s="96"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="102"/>
       <c r="AA4" s="5">
         <v>240</v>
       </c>
@@ -4448,25 +4448,25 @@
       <c r="FK4" s="1"/>
     </row>
     <row r="5" spans="1:167" s="13" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="98"/>
-      <c r="Q5" s="99"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
+      <c r="N5" s="104"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="104"/>
+      <c r="Q5" s="105"/>
       <c r="R5" s="11"/>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
@@ -4808,697 +4808,697 @@
       <c r="A8" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="106" t="s">
+      <c r="C8" s="107"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
-      <c r="K8" s="107"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="107"/>
-      <c r="N8" s="107"/>
-      <c r="O8" s="107"/>
-      <c r="P8" s="107"/>
-      <c r="Q8" s="108"/>
-      <c r="R8" s="92" t="s">
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="113"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="113"/>
+      <c r="O8" s="113"/>
+      <c r="P8" s="113"/>
+      <c r="Q8" s="114"/>
+      <c r="R8" s="98" t="s">
         <v>479</v>
       </c>
-      <c r="S8" s="93"/>
-      <c r="T8" s="93"/>
-      <c r="U8" s="93"/>
-      <c r="V8" s="93"/>
-      <c r="W8" s="93"/>
-      <c r="X8" s="93"/>
-      <c r="Y8" s="93"/>
-      <c r="Z8" s="93"/>
-      <c r="AA8" s="93"/>
-      <c r="AB8" s="93"/>
-      <c r="AC8" s="93"/>
-      <c r="AD8" s="93"/>
-      <c r="AE8" s="93"/>
-      <c r="AF8" s="93"/>
-      <c r="AG8" s="93"/>
-      <c r="AH8" s="93"/>
-      <c r="AI8" s="93"/>
-      <c r="AJ8" s="93"/>
-      <c r="AK8" s="93"/>
-      <c r="AL8" s="93"/>
-      <c r="AM8" s="93"/>
-      <c r="AN8" s="93"/>
-      <c r="AO8" s="93"/>
-      <c r="AP8" s="93"/>
-      <c r="AQ8" s="93"/>
-      <c r="AR8" s="93"/>
-      <c r="AS8" s="93"/>
-      <c r="AT8" s="93"/>
-      <c r="AU8" s="94"/>
-      <c r="AV8" s="93" t="s">
+      <c r="S8" s="99"/>
+      <c r="T8" s="99"/>
+      <c r="U8" s="99"/>
+      <c r="V8" s="99"/>
+      <c r="W8" s="99"/>
+      <c r="X8" s="99"/>
+      <c r="Y8" s="99"/>
+      <c r="Z8" s="99"/>
+      <c r="AA8" s="99"/>
+      <c r="AB8" s="99"/>
+      <c r="AC8" s="99"/>
+      <c r="AD8" s="99"/>
+      <c r="AE8" s="99"/>
+      <c r="AF8" s="99"/>
+      <c r="AG8" s="99"/>
+      <c r="AH8" s="99"/>
+      <c r="AI8" s="99"/>
+      <c r="AJ8" s="99"/>
+      <c r="AK8" s="99"/>
+      <c r="AL8" s="99"/>
+      <c r="AM8" s="99"/>
+      <c r="AN8" s="99"/>
+      <c r="AO8" s="99"/>
+      <c r="AP8" s="99"/>
+      <c r="AQ8" s="99"/>
+      <c r="AR8" s="99"/>
+      <c r="AS8" s="99"/>
+      <c r="AT8" s="99"/>
+      <c r="AU8" s="100"/>
+      <c r="AV8" s="99" t="s">
         <v>480</v>
       </c>
-      <c r="AW8" s="93"/>
-      <c r="AX8" s="93"/>
-      <c r="AY8" s="93"/>
-      <c r="AZ8" s="93"/>
-      <c r="BA8" s="93"/>
-      <c r="BB8" s="93"/>
-      <c r="BC8" s="93"/>
-      <c r="BD8" s="93"/>
-      <c r="BE8" s="93"/>
-      <c r="BF8" s="93"/>
-      <c r="BG8" s="93"/>
-      <c r="BH8" s="93"/>
-      <c r="BI8" s="93"/>
-      <c r="BJ8" s="93"/>
-      <c r="BK8" s="93"/>
-      <c r="BL8" s="93"/>
-      <c r="BM8" s="93"/>
-      <c r="BN8" s="93"/>
-      <c r="BO8" s="93"/>
-      <c r="BP8" s="93"/>
-      <c r="BQ8" s="93"/>
-      <c r="BR8" s="93"/>
-      <c r="BS8" s="93"/>
-      <c r="BT8" s="93"/>
-      <c r="BU8" s="93"/>
-      <c r="BV8" s="93"/>
-      <c r="BW8" s="93"/>
-      <c r="BX8" s="93"/>
-      <c r="BY8" s="93"/>
-      <c r="BZ8" s="93"/>
-      <c r="CA8" s="93"/>
-      <c r="CB8" s="93"/>
-      <c r="CC8" s="93"/>
-      <c r="CD8" s="93"/>
-      <c r="CE8" s="93"/>
-      <c r="CF8" s="93"/>
-      <c r="CG8" s="93"/>
-      <c r="CH8" s="93"/>
-      <c r="CI8" s="93"/>
-      <c r="CJ8" s="93"/>
-      <c r="CK8" s="93"/>
-      <c r="CL8" s="93"/>
-      <c r="CM8" s="93"/>
-      <c r="CN8" s="93"/>
-      <c r="CO8" s="93"/>
-      <c r="CP8" s="93"/>
-      <c r="CQ8" s="93"/>
-      <c r="CR8" s="93"/>
-      <c r="CS8" s="93"/>
-      <c r="CT8" s="93"/>
-      <c r="CU8" s="93"/>
-      <c r="CV8" s="93"/>
-      <c r="CW8" s="93"/>
-      <c r="CX8" s="93"/>
-      <c r="CY8" s="93"/>
-      <c r="CZ8" s="93"/>
-      <c r="DA8" s="93"/>
-      <c r="DB8" s="93"/>
-      <c r="DC8" s="93"/>
-      <c r="DD8" s="93"/>
-      <c r="DE8" s="93"/>
-      <c r="DF8" s="93"/>
-      <c r="DG8" s="93"/>
-      <c r="DH8" s="93"/>
-      <c r="DI8" s="93"/>
-      <c r="DJ8" s="93"/>
-      <c r="DK8" s="93"/>
-      <c r="DL8" s="93"/>
-      <c r="DM8" s="93"/>
-      <c r="DN8" s="93"/>
-      <c r="DO8" s="93"/>
-      <c r="DP8" s="93"/>
-      <c r="DQ8" s="93"/>
-      <c r="DR8" s="93"/>
-      <c r="DS8" s="93"/>
-      <c r="DT8" s="93"/>
-      <c r="DU8" s="93"/>
-      <c r="DV8" s="93"/>
-      <c r="DW8" s="93"/>
-      <c r="DX8" s="93"/>
-      <c r="DY8" s="93"/>
-      <c r="DZ8" s="93"/>
-      <c r="EA8" s="93"/>
-      <c r="EB8" s="93"/>
-      <c r="EC8" s="93"/>
-      <c r="ED8" s="93"/>
-      <c r="EE8" s="93"/>
-      <c r="EF8" s="93"/>
-      <c r="EG8" s="93"/>
-      <c r="EH8" s="93"/>
-      <c r="EI8" s="93"/>
-      <c r="EJ8" s="93"/>
-      <c r="EK8" s="93"/>
-      <c r="EL8" s="93"/>
-      <c r="EM8" s="93"/>
-      <c r="EN8" s="93"/>
-      <c r="EO8" s="93"/>
-      <c r="EP8" s="93"/>
-      <c r="EQ8" s="93"/>
-      <c r="ER8" s="93"/>
-      <c r="ES8" s="93"/>
-      <c r="ET8" s="93"/>
-      <c r="EU8" s="93"/>
-      <c r="EV8" s="93"/>
-      <c r="EW8" s="93"/>
-      <c r="EX8" s="93"/>
-      <c r="EY8" s="93"/>
-      <c r="EZ8" s="93"/>
-      <c r="FA8" s="93"/>
-      <c r="FB8" s="93"/>
-      <c r="FC8" s="93"/>
-      <c r="FD8" s="93"/>
-      <c r="FE8" s="93"/>
-      <c r="FF8" s="93"/>
-      <c r="FG8" s="93"/>
-      <c r="FH8" s="93"/>
-      <c r="FI8" s="93"/>
-      <c r="FJ8" s="93"/>
-      <c r="FK8" s="94"/>
+      <c r="AW8" s="99"/>
+      <c r="AX8" s="99"/>
+      <c r="AY8" s="99"/>
+      <c r="AZ8" s="99"/>
+      <c r="BA8" s="99"/>
+      <c r="BB8" s="99"/>
+      <c r="BC8" s="99"/>
+      <c r="BD8" s="99"/>
+      <c r="BE8" s="99"/>
+      <c r="BF8" s="99"/>
+      <c r="BG8" s="99"/>
+      <c r="BH8" s="99"/>
+      <c r="BI8" s="99"/>
+      <c r="BJ8" s="99"/>
+      <c r="BK8" s="99"/>
+      <c r="BL8" s="99"/>
+      <c r="BM8" s="99"/>
+      <c r="BN8" s="99"/>
+      <c r="BO8" s="99"/>
+      <c r="BP8" s="99"/>
+      <c r="BQ8" s="99"/>
+      <c r="BR8" s="99"/>
+      <c r="BS8" s="99"/>
+      <c r="BT8" s="99"/>
+      <c r="BU8" s="99"/>
+      <c r="BV8" s="99"/>
+      <c r="BW8" s="99"/>
+      <c r="BX8" s="99"/>
+      <c r="BY8" s="99"/>
+      <c r="BZ8" s="99"/>
+      <c r="CA8" s="99"/>
+      <c r="CB8" s="99"/>
+      <c r="CC8" s="99"/>
+      <c r="CD8" s="99"/>
+      <c r="CE8" s="99"/>
+      <c r="CF8" s="99"/>
+      <c r="CG8" s="99"/>
+      <c r="CH8" s="99"/>
+      <c r="CI8" s="99"/>
+      <c r="CJ8" s="99"/>
+      <c r="CK8" s="99"/>
+      <c r="CL8" s="99"/>
+      <c r="CM8" s="99"/>
+      <c r="CN8" s="99"/>
+      <c r="CO8" s="99"/>
+      <c r="CP8" s="99"/>
+      <c r="CQ8" s="99"/>
+      <c r="CR8" s="99"/>
+      <c r="CS8" s="99"/>
+      <c r="CT8" s="99"/>
+      <c r="CU8" s="99"/>
+      <c r="CV8" s="99"/>
+      <c r="CW8" s="99"/>
+      <c r="CX8" s="99"/>
+      <c r="CY8" s="99"/>
+      <c r="CZ8" s="99"/>
+      <c r="DA8" s="99"/>
+      <c r="DB8" s="99"/>
+      <c r="DC8" s="99"/>
+      <c r="DD8" s="99"/>
+      <c r="DE8" s="99"/>
+      <c r="DF8" s="99"/>
+      <c r="DG8" s="99"/>
+      <c r="DH8" s="99"/>
+      <c r="DI8" s="99"/>
+      <c r="DJ8" s="99"/>
+      <c r="DK8" s="99"/>
+      <c r="DL8" s="99"/>
+      <c r="DM8" s="99"/>
+      <c r="DN8" s="99"/>
+      <c r="DO8" s="99"/>
+      <c r="DP8" s="99"/>
+      <c r="DQ8" s="99"/>
+      <c r="DR8" s="99"/>
+      <c r="DS8" s="99"/>
+      <c r="DT8" s="99"/>
+      <c r="DU8" s="99"/>
+      <c r="DV8" s="99"/>
+      <c r="DW8" s="99"/>
+      <c r="DX8" s="99"/>
+      <c r="DY8" s="99"/>
+      <c r="DZ8" s="99"/>
+      <c r="EA8" s="99"/>
+      <c r="EB8" s="99"/>
+      <c r="EC8" s="99"/>
+      <c r="ED8" s="99"/>
+      <c r="EE8" s="99"/>
+      <c r="EF8" s="99"/>
+      <c r="EG8" s="99"/>
+      <c r="EH8" s="99"/>
+      <c r="EI8" s="99"/>
+      <c r="EJ8" s="99"/>
+      <c r="EK8" s="99"/>
+      <c r="EL8" s="99"/>
+      <c r="EM8" s="99"/>
+      <c r="EN8" s="99"/>
+      <c r="EO8" s="99"/>
+      <c r="EP8" s="99"/>
+      <c r="EQ8" s="99"/>
+      <c r="ER8" s="99"/>
+      <c r="ES8" s="99"/>
+      <c r="ET8" s="99"/>
+      <c r="EU8" s="99"/>
+      <c r="EV8" s="99"/>
+      <c r="EW8" s="99"/>
+      <c r="EX8" s="99"/>
+      <c r="EY8" s="99"/>
+      <c r="EZ8" s="99"/>
+      <c r="FA8" s="99"/>
+      <c r="FB8" s="99"/>
+      <c r="FC8" s="99"/>
+      <c r="FD8" s="99"/>
+      <c r="FE8" s="99"/>
+      <c r="FF8" s="99"/>
+      <c r="FG8" s="99"/>
+      <c r="FH8" s="99"/>
+      <c r="FI8" s="99"/>
+      <c r="FJ8" s="99"/>
+      <c r="FK8" s="100"/>
     </row>
     <row r="9" spans="1:167" s="18" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="75"/>
-      <c r="B9" s="103"/>
-      <c r="C9" s="104"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="110"/>
-      <c r="N9" s="110"/>
-      <c r="O9" s="110"/>
-      <c r="P9" s="110"/>
-      <c r="Q9" s="111"/>
-      <c r="R9" s="118" t="str">
+      <c r="B9" s="109"/>
+      <c r="C9" s="110"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="116"/>
+      <c r="H9" s="116"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116"/>
+      <c r="M9" s="116"/>
+      <c r="N9" s="116"/>
+      <c r="O9" s="116"/>
+      <c r="P9" s="116"/>
+      <c r="Q9" s="117"/>
+      <c r="R9" s="91" t="str">
         <f>UPPER(TEXT(R10,"DDDD"))</f>
         <v>LUNES</v>
       </c>
-      <c r="S9" s="119"/>
-      <c r="T9" s="119"/>
-      <c r="U9" s="119"/>
-      <c r="V9" s="120"/>
-      <c r="W9" s="118" t="str">
+      <c r="S9" s="92"/>
+      <c r="T9" s="92"/>
+      <c r="U9" s="92"/>
+      <c r="V9" s="93"/>
+      <c r="W9" s="91" t="str">
         <f t="shared" ref="W9" si="0">UPPER(TEXT(W10,"DDDD"))</f>
         <v>MARTES</v>
       </c>
-      <c r="X9" s="119"/>
-      <c r="Y9" s="119"/>
-      <c r="Z9" s="119"/>
-      <c r="AA9" s="120"/>
-      <c r="AB9" s="118" t="str">
+      <c r="X9" s="92"/>
+      <c r="Y9" s="92"/>
+      <c r="Z9" s="92"/>
+      <c r="AA9" s="93"/>
+      <c r="AB9" s="91" t="str">
         <f t="shared" ref="AB9" si="1">UPPER(TEXT(AB10,"DDDD"))</f>
         <v>MIÉRCOLES</v>
       </c>
-      <c r="AC9" s="119"/>
-      <c r="AD9" s="119"/>
-      <c r="AE9" s="119"/>
-      <c r="AF9" s="120"/>
-      <c r="AG9" s="118" t="str">
+      <c r="AC9" s="92"/>
+      <c r="AD9" s="92"/>
+      <c r="AE9" s="92"/>
+      <c r="AF9" s="93"/>
+      <c r="AG9" s="91" t="str">
         <f t="shared" ref="AG9" si="2">UPPER(TEXT(AG10,"DDDD"))</f>
         <v>JUEVES</v>
       </c>
-      <c r="AH9" s="119"/>
-      <c r="AI9" s="119"/>
-      <c r="AJ9" s="119"/>
-      <c r="AK9" s="120"/>
-      <c r="AL9" s="118" t="str">
+      <c r="AH9" s="92"/>
+      <c r="AI9" s="92"/>
+      <c r="AJ9" s="92"/>
+      <c r="AK9" s="93"/>
+      <c r="AL9" s="91" t="str">
         <f t="shared" ref="AL9" si="3">UPPER(TEXT(AL10,"DDDD"))</f>
         <v>VIERNES</v>
       </c>
-      <c r="AM9" s="119"/>
-      <c r="AN9" s="119"/>
-      <c r="AO9" s="119"/>
-      <c r="AP9" s="120"/>
-      <c r="AQ9" s="118" t="str">
+      <c r="AM9" s="92"/>
+      <c r="AN9" s="92"/>
+      <c r="AO9" s="92"/>
+      <c r="AP9" s="93"/>
+      <c r="AQ9" s="91" t="str">
         <f t="shared" ref="AQ9" si="4">UPPER(TEXT(AQ10,"DDDD"))</f>
         <v>SÁBADO</v>
       </c>
-      <c r="AR9" s="119"/>
-      <c r="AS9" s="119"/>
-      <c r="AT9" s="119"/>
-      <c r="AU9" s="120"/>
-      <c r="AV9" s="118" t="str">
+      <c r="AR9" s="92"/>
+      <c r="AS9" s="92"/>
+      <c r="AT9" s="92"/>
+      <c r="AU9" s="93"/>
+      <c r="AV9" s="91" t="str">
         <f t="shared" ref="AV9" si="5">UPPER(TEXT(AV10,"DDDD"))</f>
         <v>DOMINGO</v>
       </c>
-      <c r="AW9" s="119"/>
-      <c r="AX9" s="119"/>
-      <c r="AY9" s="119"/>
-      <c r="AZ9" s="120"/>
-      <c r="BA9" s="118" t="str">
+      <c r="AW9" s="92"/>
+      <c r="AX9" s="92"/>
+      <c r="AY9" s="92"/>
+      <c r="AZ9" s="93"/>
+      <c r="BA9" s="91" t="str">
         <f t="shared" ref="BA9" si="6">UPPER(TEXT(BA10,"DDDD"))</f>
         <v>LUNES</v>
       </c>
-      <c r="BB9" s="119"/>
-      <c r="BC9" s="119"/>
-      <c r="BD9" s="119"/>
-      <c r="BE9" s="120"/>
-      <c r="BF9" s="118" t="str">
+      <c r="BB9" s="92"/>
+      <c r="BC9" s="92"/>
+      <c r="BD9" s="92"/>
+      <c r="BE9" s="93"/>
+      <c r="BF9" s="91" t="str">
         <f t="shared" ref="BF9" si="7">UPPER(TEXT(BF10,"DDDD"))</f>
         <v>MARTES</v>
       </c>
-      <c r="BG9" s="119"/>
-      <c r="BH9" s="119"/>
-      <c r="BI9" s="119"/>
-      <c r="BJ9" s="120"/>
-      <c r="BK9" s="118" t="str">
+      <c r="BG9" s="92"/>
+      <c r="BH9" s="92"/>
+      <c r="BI9" s="92"/>
+      <c r="BJ9" s="93"/>
+      <c r="BK9" s="91" t="str">
         <f t="shared" ref="BK9" si="8">UPPER(TEXT(BK10,"DDDD"))</f>
         <v>MIÉRCOLES</v>
       </c>
-      <c r="BL9" s="119"/>
-      <c r="BM9" s="119"/>
-      <c r="BN9" s="119"/>
-      <c r="BO9" s="120"/>
-      <c r="BP9" s="118" t="str">
+      <c r="BL9" s="92"/>
+      <c r="BM9" s="92"/>
+      <c r="BN9" s="92"/>
+      <c r="BO9" s="93"/>
+      <c r="BP9" s="91" t="str">
         <f t="shared" ref="BP9" si="9">UPPER(TEXT(BP10,"DDDD"))</f>
         <v>JUEVES</v>
       </c>
-      <c r="BQ9" s="119"/>
-      <c r="BR9" s="119"/>
-      <c r="BS9" s="119"/>
-      <c r="BT9" s="120"/>
-      <c r="BU9" s="118" t="str">
+      <c r="BQ9" s="92"/>
+      <c r="BR9" s="92"/>
+      <c r="BS9" s="92"/>
+      <c r="BT9" s="93"/>
+      <c r="BU9" s="91" t="str">
         <f t="shared" ref="BU9" si="10">UPPER(TEXT(BU10,"DDDD"))</f>
         <v>VIERNES</v>
       </c>
-      <c r="BV9" s="119"/>
-      <c r="BW9" s="119"/>
-      <c r="BX9" s="119"/>
-      <c r="BY9" s="120"/>
-      <c r="BZ9" s="118" t="str">
+      <c r="BV9" s="92"/>
+      <c r="BW9" s="92"/>
+      <c r="BX9" s="92"/>
+      <c r="BY9" s="93"/>
+      <c r="BZ9" s="91" t="str">
         <f t="shared" ref="BZ9" si="11">UPPER(TEXT(BZ10,"DDDD"))</f>
         <v>SÁBADO</v>
       </c>
-      <c r="CA9" s="119"/>
-      <c r="CB9" s="119"/>
-      <c r="CC9" s="119"/>
-      <c r="CD9" s="120"/>
-      <c r="CE9" s="118" t="str">
+      <c r="CA9" s="92"/>
+      <c r="CB9" s="92"/>
+      <c r="CC9" s="92"/>
+      <c r="CD9" s="93"/>
+      <c r="CE9" s="91" t="str">
         <f t="shared" ref="CE9" si="12">UPPER(TEXT(CE10,"DDDD"))</f>
         <v>DOMINGO</v>
       </c>
-      <c r="CF9" s="119"/>
-      <c r="CG9" s="119"/>
-      <c r="CH9" s="119"/>
-      <c r="CI9" s="120"/>
-      <c r="CJ9" s="118" t="str">
+      <c r="CF9" s="92"/>
+      <c r="CG9" s="92"/>
+      <c r="CH9" s="92"/>
+      <c r="CI9" s="93"/>
+      <c r="CJ9" s="91" t="str">
         <f t="shared" ref="CJ9" si="13">UPPER(TEXT(CJ10,"DDDD"))</f>
         <v>LUNES</v>
       </c>
-      <c r="CK9" s="119"/>
-      <c r="CL9" s="119"/>
-      <c r="CM9" s="119"/>
-      <c r="CN9" s="120"/>
-      <c r="CO9" s="118" t="str">
+      <c r="CK9" s="92"/>
+      <c r="CL9" s="92"/>
+      <c r="CM9" s="92"/>
+      <c r="CN9" s="93"/>
+      <c r="CO9" s="91" t="str">
         <f t="shared" ref="CO9" si="14">UPPER(TEXT(CO10,"DDDD"))</f>
         <v>MARTES</v>
       </c>
-      <c r="CP9" s="119"/>
-      <c r="CQ9" s="119"/>
-      <c r="CR9" s="119"/>
-      <c r="CS9" s="120"/>
-      <c r="CT9" s="118" t="str">
+      <c r="CP9" s="92"/>
+      <c r="CQ9" s="92"/>
+      <c r="CR9" s="92"/>
+      <c r="CS9" s="93"/>
+      <c r="CT9" s="91" t="str">
         <f t="shared" ref="CT9" si="15">UPPER(TEXT(CT10,"DDDD"))</f>
         <v>MIÉRCOLES</v>
       </c>
-      <c r="CU9" s="119"/>
-      <c r="CV9" s="119"/>
-      <c r="CW9" s="119"/>
-      <c r="CX9" s="120"/>
-      <c r="CY9" s="118" t="str">
+      <c r="CU9" s="92"/>
+      <c r="CV9" s="92"/>
+      <c r="CW9" s="92"/>
+      <c r="CX9" s="93"/>
+      <c r="CY9" s="91" t="str">
         <f t="shared" ref="CY9" si="16">UPPER(TEXT(CY10,"DDDD"))</f>
         <v>JUEVES</v>
       </c>
-      <c r="CZ9" s="119"/>
-      <c r="DA9" s="119"/>
-      <c r="DB9" s="119"/>
-      <c r="DC9" s="120"/>
-      <c r="DD9" s="118" t="str">
+      <c r="CZ9" s="92"/>
+      <c r="DA9" s="92"/>
+      <c r="DB9" s="92"/>
+      <c r="DC9" s="93"/>
+      <c r="DD9" s="91" t="str">
         <f t="shared" ref="DD9" si="17">UPPER(TEXT(DD10,"DDDD"))</f>
         <v>VIERNES</v>
       </c>
-      <c r="DE9" s="119"/>
-      <c r="DF9" s="119"/>
-      <c r="DG9" s="119"/>
-      <c r="DH9" s="120"/>
-      <c r="DI9" s="118" t="str">
+      <c r="DE9" s="92"/>
+      <c r="DF9" s="92"/>
+      <c r="DG9" s="92"/>
+      <c r="DH9" s="93"/>
+      <c r="DI9" s="91" t="str">
         <f t="shared" ref="DI9" si="18">UPPER(TEXT(DI10,"DDDD"))</f>
         <v>SÁBADO</v>
       </c>
-      <c r="DJ9" s="119"/>
-      <c r="DK9" s="119"/>
-      <c r="DL9" s="119"/>
-      <c r="DM9" s="120"/>
-      <c r="DN9" s="118" t="str">
+      <c r="DJ9" s="92"/>
+      <c r="DK9" s="92"/>
+      <c r="DL9" s="92"/>
+      <c r="DM9" s="93"/>
+      <c r="DN9" s="91" t="str">
         <f t="shared" ref="DN9" si="19">UPPER(TEXT(DN10,"DDDD"))</f>
         <v>DOMINGO</v>
       </c>
-      <c r="DO9" s="119"/>
-      <c r="DP9" s="119"/>
-      <c r="DQ9" s="119"/>
-      <c r="DR9" s="120"/>
-      <c r="DS9" s="118" t="str">
+      <c r="DO9" s="92"/>
+      <c r="DP9" s="92"/>
+      <c r="DQ9" s="92"/>
+      <c r="DR9" s="93"/>
+      <c r="DS9" s="91" t="str">
         <f t="shared" ref="DS9" si="20">UPPER(TEXT(DS10,"DDDD"))</f>
         <v>LUNES</v>
       </c>
-      <c r="DT9" s="119"/>
-      <c r="DU9" s="119"/>
-      <c r="DV9" s="119"/>
-      <c r="DW9" s="120"/>
-      <c r="DX9" s="118" t="str">
+      <c r="DT9" s="92"/>
+      <c r="DU9" s="92"/>
+      <c r="DV9" s="92"/>
+      <c r="DW9" s="93"/>
+      <c r="DX9" s="91" t="str">
         <f t="shared" ref="DX9" si="21">UPPER(TEXT(DX10,"DDDD"))</f>
         <v>MARTES</v>
       </c>
-      <c r="DY9" s="119"/>
-      <c r="DZ9" s="119"/>
-      <c r="EA9" s="119"/>
-      <c r="EB9" s="120"/>
-      <c r="EC9" s="118" t="str">
+      <c r="DY9" s="92"/>
+      <c r="DZ9" s="92"/>
+      <c r="EA9" s="92"/>
+      <c r="EB9" s="93"/>
+      <c r="EC9" s="91" t="str">
         <f t="shared" ref="EC9" si="22">UPPER(TEXT(EC10,"DDDD"))</f>
         <v>MIÉRCOLES</v>
       </c>
-      <c r="ED9" s="119"/>
-      <c r="EE9" s="119"/>
-      <c r="EF9" s="119"/>
-      <c r="EG9" s="120"/>
-      <c r="EH9" s="118" t="str">
+      <c r="ED9" s="92"/>
+      <c r="EE9" s="92"/>
+      <c r="EF9" s="92"/>
+      <c r="EG9" s="93"/>
+      <c r="EH9" s="91" t="str">
         <f t="shared" ref="EH9" si="23">UPPER(TEXT(EH10,"DDDD"))</f>
         <v>JUEVES</v>
       </c>
-      <c r="EI9" s="119"/>
-      <c r="EJ9" s="119"/>
-      <c r="EK9" s="119"/>
-      <c r="EL9" s="120"/>
-      <c r="EM9" s="118" t="str">
+      <c r="EI9" s="92"/>
+      <c r="EJ9" s="92"/>
+      <c r="EK9" s="92"/>
+      <c r="EL9" s="93"/>
+      <c r="EM9" s="91" t="str">
         <f t="shared" ref="EM9" si="24">UPPER(TEXT(EM10,"DDDD"))</f>
         <v>VIERNES</v>
       </c>
-      <c r="EN9" s="119"/>
-      <c r="EO9" s="119"/>
-      <c r="EP9" s="119"/>
-      <c r="EQ9" s="120"/>
-      <c r="ER9" s="118" t="str">
+      <c r="EN9" s="92"/>
+      <c r="EO9" s="92"/>
+      <c r="EP9" s="92"/>
+      <c r="EQ9" s="93"/>
+      <c r="ER9" s="91" t="str">
         <f t="shared" ref="ER9" si="25">UPPER(TEXT(ER10,"DDDD"))</f>
         <v>SÁBADO</v>
       </c>
-      <c r="ES9" s="119"/>
-      <c r="ET9" s="119"/>
-      <c r="EU9" s="119"/>
-      <c r="EV9" s="120"/>
-      <c r="EW9" s="118" t="str">
+      <c r="ES9" s="92"/>
+      <c r="ET9" s="92"/>
+      <c r="EU9" s="92"/>
+      <c r="EV9" s="93"/>
+      <c r="EW9" s="91" t="str">
         <f t="shared" ref="EW9" si="26">UPPER(TEXT(EW10,"DDDD"))</f>
         <v>DOMINGO</v>
       </c>
-      <c r="EX9" s="119"/>
-      <c r="EY9" s="119"/>
-      <c r="EZ9" s="119"/>
-      <c r="FA9" s="120"/>
-      <c r="FB9" s="118" t="str">
+      <c r="EX9" s="92"/>
+      <c r="EY9" s="92"/>
+      <c r="EZ9" s="92"/>
+      <c r="FA9" s="93"/>
+      <c r="FB9" s="91" t="str">
         <f t="shared" ref="FB9" si="27">UPPER(TEXT(FB10,"DDDD"))</f>
         <v>LUNES</v>
       </c>
-      <c r="FC9" s="119"/>
-      <c r="FD9" s="119"/>
-      <c r="FE9" s="119"/>
-      <c r="FF9" s="120"/>
-      <c r="FG9" s="118" t="str">
+      <c r="FC9" s="92"/>
+      <c r="FD9" s="92"/>
+      <c r="FE9" s="92"/>
+      <c r="FF9" s="93"/>
+      <c r="FG9" s="91" t="str">
         <f t="shared" ref="FG9" si="28">UPPER(TEXT(FG10,"DDDD"))</f>
         <v>MARTES</v>
       </c>
-      <c r="FH9" s="119"/>
-      <c r="FI9" s="119"/>
-      <c r="FJ9" s="119"/>
-      <c r="FK9" s="120"/>
+      <c r="FH9" s="92"/>
+      <c r="FI9" s="92"/>
+      <c r="FJ9" s="92"/>
+      <c r="FK9" s="93"/>
     </row>
     <row r="10" spans="1:167" s="12" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="75"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="104"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="113"/>
-      <c r="H10" s="113"/>
-      <c r="I10" s="113"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="113"/>
-      <c r="N10" s="113"/>
-      <c r="O10" s="113"/>
-      <c r="P10" s="113"/>
-      <c r="Q10" s="114"/>
-      <c r="R10" s="115">
+      <c r="B10" s="109"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="119"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="119"/>
+      <c r="Q10" s="120"/>
+      <c r="R10" s="88">
         <v>44676</v>
       </c>
-      <c r="S10" s="116"/>
-      <c r="T10" s="116"/>
-      <c r="U10" s="116"/>
-      <c r="V10" s="117"/>
-      <c r="W10" s="115">
+      <c r="S10" s="89"/>
+      <c r="T10" s="89"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="90"/>
+      <c r="W10" s="88">
         <f>+R10+1</f>
         <v>44677</v>
       </c>
-      <c r="X10" s="116"/>
-      <c r="Y10" s="116"/>
-      <c r="Z10" s="116"/>
-      <c r="AA10" s="117"/>
-      <c r="AB10" s="115">
+      <c r="X10" s="89"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="89"/>
+      <c r="AA10" s="90"/>
+      <c r="AB10" s="88">
         <f t="shared" ref="AB10" si="29">+W10+1</f>
         <v>44678</v>
       </c>
-      <c r="AC10" s="116"/>
-      <c r="AD10" s="116"/>
-      <c r="AE10" s="116"/>
-      <c r="AF10" s="117"/>
-      <c r="AG10" s="115">
+      <c r="AC10" s="89"/>
+      <c r="AD10" s="89"/>
+      <c r="AE10" s="89"/>
+      <c r="AF10" s="90"/>
+      <c r="AG10" s="88">
         <f t="shared" ref="AG10" si="30">+AB10+1</f>
         <v>44679</v>
       </c>
-      <c r="AH10" s="116"/>
-      <c r="AI10" s="116"/>
-      <c r="AJ10" s="116"/>
-      <c r="AK10" s="117"/>
-      <c r="AL10" s="115">
+      <c r="AH10" s="89"/>
+      <c r="AI10" s="89"/>
+      <c r="AJ10" s="89"/>
+      <c r="AK10" s="90"/>
+      <c r="AL10" s="88">
         <f t="shared" ref="AL10" si="31">+AG10+1</f>
         <v>44680</v>
       </c>
-      <c r="AM10" s="116"/>
-      <c r="AN10" s="116"/>
-      <c r="AO10" s="116"/>
-      <c r="AP10" s="117"/>
-      <c r="AQ10" s="115">
+      <c r="AM10" s="89"/>
+      <c r="AN10" s="89"/>
+      <c r="AO10" s="89"/>
+      <c r="AP10" s="90"/>
+      <c r="AQ10" s="88">
         <f t="shared" ref="AQ10" si="32">+AL10+1</f>
         <v>44681</v>
       </c>
-      <c r="AR10" s="116"/>
-      <c r="AS10" s="116"/>
-      <c r="AT10" s="116"/>
-      <c r="AU10" s="117"/>
-      <c r="AV10" s="115">
+      <c r="AR10" s="89"/>
+      <c r="AS10" s="89"/>
+      <c r="AT10" s="89"/>
+      <c r="AU10" s="90"/>
+      <c r="AV10" s="88">
         <f t="shared" ref="AV10" si="33">+AQ10+1</f>
         <v>44682</v>
       </c>
-      <c r="AW10" s="116"/>
-      <c r="AX10" s="116"/>
-      <c r="AY10" s="116"/>
-      <c r="AZ10" s="117"/>
-      <c r="BA10" s="115">
+      <c r="AW10" s="89"/>
+      <c r="AX10" s="89"/>
+      <c r="AY10" s="89"/>
+      <c r="AZ10" s="90"/>
+      <c r="BA10" s="88">
         <f t="shared" ref="BA10" si="34">+AV10+1</f>
         <v>44683</v>
       </c>
-      <c r="BB10" s="116"/>
-      <c r="BC10" s="116"/>
-      <c r="BD10" s="116"/>
-      <c r="BE10" s="117"/>
-      <c r="BF10" s="115">
+      <c r="BB10" s="89"/>
+      <c r="BC10" s="89"/>
+      <c r="BD10" s="89"/>
+      <c r="BE10" s="90"/>
+      <c r="BF10" s="88">
         <f t="shared" ref="BF10" si="35">+BA10+1</f>
         <v>44684</v>
       </c>
-      <c r="BG10" s="116"/>
-      <c r="BH10" s="116"/>
-      <c r="BI10" s="116"/>
-      <c r="BJ10" s="117"/>
-      <c r="BK10" s="115">
+      <c r="BG10" s="89"/>
+      <c r="BH10" s="89"/>
+      <c r="BI10" s="89"/>
+      <c r="BJ10" s="90"/>
+      <c r="BK10" s="88">
         <f t="shared" ref="BK10" si="36">+BF10+1</f>
         <v>44685</v>
       </c>
-      <c r="BL10" s="116"/>
-      <c r="BM10" s="116"/>
-      <c r="BN10" s="116"/>
-      <c r="BO10" s="117"/>
-      <c r="BP10" s="115">
+      <c r="BL10" s="89"/>
+      <c r="BM10" s="89"/>
+      <c r="BN10" s="89"/>
+      <c r="BO10" s="90"/>
+      <c r="BP10" s="88">
         <f t="shared" ref="BP10" si="37">+BK10+1</f>
         <v>44686</v>
       </c>
-      <c r="BQ10" s="116"/>
-      <c r="BR10" s="116"/>
-      <c r="BS10" s="116"/>
-      <c r="BT10" s="117"/>
-      <c r="BU10" s="115">
+      <c r="BQ10" s="89"/>
+      <c r="BR10" s="89"/>
+      <c r="BS10" s="89"/>
+      <c r="BT10" s="90"/>
+      <c r="BU10" s="88">
         <f t="shared" ref="BU10" si="38">+BP10+1</f>
         <v>44687</v>
       </c>
-      <c r="BV10" s="116"/>
-      <c r="BW10" s="116"/>
-      <c r="BX10" s="116"/>
-      <c r="BY10" s="117"/>
-      <c r="BZ10" s="115">
+      <c r="BV10" s="89"/>
+      <c r="BW10" s="89"/>
+      <c r="BX10" s="89"/>
+      <c r="BY10" s="90"/>
+      <c r="BZ10" s="88">
         <f t="shared" ref="BZ10" si="39">+BU10+1</f>
         <v>44688</v>
       </c>
-      <c r="CA10" s="116"/>
-      <c r="CB10" s="116"/>
-      <c r="CC10" s="116"/>
-      <c r="CD10" s="117"/>
-      <c r="CE10" s="115">
+      <c r="CA10" s="89"/>
+      <c r="CB10" s="89"/>
+      <c r="CC10" s="89"/>
+      <c r="CD10" s="90"/>
+      <c r="CE10" s="88">
         <f t="shared" ref="CE10" si="40">+BZ10+1</f>
         <v>44689</v>
       </c>
-      <c r="CF10" s="116"/>
-      <c r="CG10" s="116"/>
-      <c r="CH10" s="116"/>
-      <c r="CI10" s="117"/>
-      <c r="CJ10" s="115">
+      <c r="CF10" s="89"/>
+      <c r="CG10" s="89"/>
+      <c r="CH10" s="89"/>
+      <c r="CI10" s="90"/>
+      <c r="CJ10" s="88">
         <f t="shared" ref="CJ10" si="41">+CE10+1</f>
         <v>44690</v>
       </c>
-      <c r="CK10" s="116"/>
-      <c r="CL10" s="116"/>
-      <c r="CM10" s="116"/>
-      <c r="CN10" s="117"/>
-      <c r="CO10" s="115">
+      <c r="CK10" s="89"/>
+      <c r="CL10" s="89"/>
+      <c r="CM10" s="89"/>
+      <c r="CN10" s="90"/>
+      <c r="CO10" s="88">
         <f t="shared" ref="CO10" si="42">+CJ10+1</f>
         <v>44691</v>
       </c>
-      <c r="CP10" s="116"/>
-      <c r="CQ10" s="116"/>
-      <c r="CR10" s="116"/>
-      <c r="CS10" s="117"/>
-      <c r="CT10" s="115">
+      <c r="CP10" s="89"/>
+      <c r="CQ10" s="89"/>
+      <c r="CR10" s="89"/>
+      <c r="CS10" s="90"/>
+      <c r="CT10" s="88">
         <f t="shared" ref="CT10" si="43">+CO10+1</f>
         <v>44692</v>
       </c>
-      <c r="CU10" s="116"/>
-      <c r="CV10" s="116"/>
-      <c r="CW10" s="116"/>
-      <c r="CX10" s="117"/>
-      <c r="CY10" s="115">
+      <c r="CU10" s="89"/>
+      <c r="CV10" s="89"/>
+      <c r="CW10" s="89"/>
+      <c r="CX10" s="90"/>
+      <c r="CY10" s="88">
         <f t="shared" ref="CY10" si="44">+CT10+1</f>
         <v>44693</v>
       </c>
-      <c r="CZ10" s="116"/>
-      <c r="DA10" s="116"/>
-      <c r="DB10" s="116"/>
-      <c r="DC10" s="117"/>
-      <c r="DD10" s="115">
+      <c r="CZ10" s="89"/>
+      <c r="DA10" s="89"/>
+      <c r="DB10" s="89"/>
+      <c r="DC10" s="90"/>
+      <c r="DD10" s="88">
         <f t="shared" ref="DD10" si="45">+CY10+1</f>
         <v>44694</v>
       </c>
-      <c r="DE10" s="116"/>
-      <c r="DF10" s="116"/>
-      <c r="DG10" s="116"/>
-      <c r="DH10" s="117"/>
-      <c r="DI10" s="115">
+      <c r="DE10" s="89"/>
+      <c r="DF10" s="89"/>
+      <c r="DG10" s="89"/>
+      <c r="DH10" s="90"/>
+      <c r="DI10" s="88">
         <f t="shared" ref="DI10" si="46">+DD10+1</f>
         <v>44695</v>
       </c>
-      <c r="DJ10" s="116"/>
-      <c r="DK10" s="116"/>
-      <c r="DL10" s="116"/>
-      <c r="DM10" s="117"/>
-      <c r="DN10" s="115">
+      <c r="DJ10" s="89"/>
+      <c r="DK10" s="89"/>
+      <c r="DL10" s="89"/>
+      <c r="DM10" s="90"/>
+      <c r="DN10" s="88">
         <f t="shared" ref="DN10" si="47">+DI10+1</f>
         <v>44696</v>
       </c>
-      <c r="DO10" s="116"/>
-      <c r="DP10" s="116"/>
-      <c r="DQ10" s="116"/>
-      <c r="DR10" s="117"/>
-      <c r="DS10" s="115">
+      <c r="DO10" s="89"/>
+      <c r="DP10" s="89"/>
+      <c r="DQ10" s="89"/>
+      <c r="DR10" s="90"/>
+      <c r="DS10" s="88">
         <f t="shared" ref="DS10" si="48">+DN10+1</f>
         <v>44697</v>
       </c>
-      <c r="DT10" s="116"/>
-      <c r="DU10" s="116"/>
-      <c r="DV10" s="116"/>
-      <c r="DW10" s="117"/>
-      <c r="DX10" s="115">
+      <c r="DT10" s="89"/>
+      <c r="DU10" s="89"/>
+      <c r="DV10" s="89"/>
+      <c r="DW10" s="90"/>
+      <c r="DX10" s="88">
         <f t="shared" ref="DX10" si="49">+DS10+1</f>
         <v>44698</v>
       </c>
-      <c r="DY10" s="116"/>
-      <c r="DZ10" s="116"/>
-      <c r="EA10" s="116"/>
-      <c r="EB10" s="117"/>
-      <c r="EC10" s="115">
+      <c r="DY10" s="89"/>
+      <c r="DZ10" s="89"/>
+      <c r="EA10" s="89"/>
+      <c r="EB10" s="90"/>
+      <c r="EC10" s="88">
         <f t="shared" ref="EC10" si="50">+DX10+1</f>
         <v>44699</v>
       </c>
-      <c r="ED10" s="116"/>
-      <c r="EE10" s="116"/>
-      <c r="EF10" s="116"/>
-      <c r="EG10" s="117"/>
-      <c r="EH10" s="115">
+      <c r="ED10" s="89"/>
+      <c r="EE10" s="89"/>
+      <c r="EF10" s="89"/>
+      <c r="EG10" s="90"/>
+      <c r="EH10" s="88">
         <f t="shared" ref="EH10" si="51">+EC10+1</f>
         <v>44700</v>
       </c>
-      <c r="EI10" s="116"/>
-      <c r="EJ10" s="116"/>
-      <c r="EK10" s="116"/>
-      <c r="EL10" s="117"/>
-      <c r="EM10" s="115">
+      <c r="EI10" s="89"/>
+      <c r="EJ10" s="89"/>
+      <c r="EK10" s="89"/>
+      <c r="EL10" s="90"/>
+      <c r="EM10" s="88">
         <f t="shared" ref="EM10" si="52">+EH10+1</f>
         <v>44701</v>
       </c>
-      <c r="EN10" s="116"/>
-      <c r="EO10" s="116"/>
-      <c r="EP10" s="116"/>
-      <c r="EQ10" s="117"/>
-      <c r="ER10" s="115">
+      <c r="EN10" s="89"/>
+      <c r="EO10" s="89"/>
+      <c r="EP10" s="89"/>
+      <c r="EQ10" s="90"/>
+      <c r="ER10" s="88">
         <f t="shared" ref="ER10" si="53">+EM10+1</f>
         <v>44702</v>
       </c>
-      <c r="ES10" s="116"/>
-      <c r="ET10" s="116"/>
-      <c r="EU10" s="116"/>
-      <c r="EV10" s="117"/>
-      <c r="EW10" s="115">
+      <c r="ES10" s="89"/>
+      <c r="ET10" s="89"/>
+      <c r="EU10" s="89"/>
+      <c r="EV10" s="90"/>
+      <c r="EW10" s="88">
         <f t="shared" ref="EW10" si="54">+ER10+1</f>
         <v>44703</v>
       </c>
-      <c r="EX10" s="116"/>
-      <c r="EY10" s="116"/>
-      <c r="EZ10" s="116"/>
-      <c r="FA10" s="117"/>
-      <c r="FB10" s="115">
+      <c r="EX10" s="89"/>
+      <c r="EY10" s="89"/>
+      <c r="EZ10" s="89"/>
+      <c r="FA10" s="90"/>
+      <c r="FB10" s="88">
         <f t="shared" ref="FB10" si="55">+EW10+1</f>
         <v>44704</v>
       </c>
-      <c r="FC10" s="116"/>
-      <c r="FD10" s="116"/>
-      <c r="FE10" s="116"/>
-      <c r="FF10" s="117"/>
-      <c r="FG10" s="115">
+      <c r="FC10" s="89"/>
+      <c r="FD10" s="89"/>
+      <c r="FE10" s="89"/>
+      <c r="FF10" s="90"/>
+      <c r="FG10" s="88">
         <f t="shared" ref="FG10" si="56">+FB10+1</f>
         <v>44705</v>
       </c>
-      <c r="FH10" s="116"/>
-      <c r="FI10" s="116"/>
-      <c r="FJ10" s="116"/>
-      <c r="FK10" s="117"/>
+      <c r="FH10" s="89"/>
+      <c r="FI10" s="89"/>
+      <c r="FJ10" s="89"/>
+      <c r="FK10" s="90"/>
     </row>
     <row r="11" spans="1:167" s="21" customFormat="1" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="75"/>
@@ -8541,7 +8541,7 @@
       <c r="FJ20" s="35"/>
       <c r="FK20" s="36"/>
     </row>
-    <row r="21" spans="1:167" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:167" s="4" customFormat="1" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>25</v>
       </c>
@@ -20391,7 +20391,7 @@
       <c r="FJ61" s="35"/>
       <c r="FK61" s="36"/>
     </row>
-    <row r="62" spans="1:167" s="4" customFormat="1" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:167" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>66</v>
       </c>
@@ -47317,66 +47317,11 @@
   <autoFilter ref="A11:FK150" xr:uid="{C0760EAB-CC3D-40AE-A29A-AB65FF61DEFD}">
     <filterColumn colId="1">
       <filters>
-        <filter val="ATAHUA LINARES"/>
+        <filter val="FARFAN FAJARDO"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="71">
-    <mergeCell ref="FG10:FK10"/>
-    <mergeCell ref="DN10:DR10"/>
-    <mergeCell ref="DS10:DW10"/>
-    <mergeCell ref="DX10:EB10"/>
-    <mergeCell ref="EC10:EG10"/>
-    <mergeCell ref="EH10:EL10"/>
-    <mergeCell ref="EM10:EQ10"/>
-    <mergeCell ref="EW10:FA10"/>
-    <mergeCell ref="FB10:FF10"/>
-    <mergeCell ref="ER10:EV10"/>
-    <mergeCell ref="AB10:AF10"/>
-    <mergeCell ref="AG10:AK10"/>
-    <mergeCell ref="AL10:AP10"/>
-    <mergeCell ref="DI10:DM10"/>
-    <mergeCell ref="BF10:BJ10"/>
-    <mergeCell ref="BK10:BO10"/>
-    <mergeCell ref="BP10:BT10"/>
-    <mergeCell ref="BU10:BY10"/>
-    <mergeCell ref="AQ10:AU10"/>
-    <mergeCell ref="AV10:AZ10"/>
-    <mergeCell ref="BA10:BE10"/>
-    <mergeCell ref="DD9:DH9"/>
-    <mergeCell ref="DI9:DM9"/>
-    <mergeCell ref="DN9:DR9"/>
-    <mergeCell ref="DS9:DW9"/>
-    <mergeCell ref="DD10:DH10"/>
-    <mergeCell ref="FG9:FK9"/>
-    <mergeCell ref="EC9:EG9"/>
-    <mergeCell ref="EH9:EL9"/>
-    <mergeCell ref="EM9:EQ9"/>
-    <mergeCell ref="ER9:EV9"/>
-    <mergeCell ref="EW9:FA9"/>
-    <mergeCell ref="FB9:FF9"/>
-    <mergeCell ref="AB9:AF9"/>
-    <mergeCell ref="AG9:AK9"/>
-    <mergeCell ref="AL9:AP9"/>
-    <mergeCell ref="BF9:BJ9"/>
-    <mergeCell ref="BK9:BO9"/>
-    <mergeCell ref="AQ9:AU9"/>
-    <mergeCell ref="AV9:AZ9"/>
-    <mergeCell ref="BA9:BE9"/>
-    <mergeCell ref="BU9:BY9"/>
-    <mergeCell ref="BZ9:CD9"/>
-    <mergeCell ref="BZ10:CD10"/>
-    <mergeCell ref="BP9:BT9"/>
-    <mergeCell ref="CY9:DC9"/>
-    <mergeCell ref="CJ10:CN10"/>
-    <mergeCell ref="CE10:CI10"/>
-    <mergeCell ref="CO10:CS10"/>
-    <mergeCell ref="CT10:CX10"/>
-    <mergeCell ref="CY10:DC10"/>
-    <mergeCell ref="CE9:CI9"/>
-    <mergeCell ref="CJ9:CN9"/>
-    <mergeCell ref="CO9:CS9"/>
-    <mergeCell ref="CT9:CX9"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:Q3"/>
@@ -47393,6 +47338,61 @@
     <mergeCell ref="R9:V9"/>
     <mergeCell ref="W9:AA9"/>
     <mergeCell ref="DX9:EB9"/>
+    <mergeCell ref="BU9:BY9"/>
+    <mergeCell ref="BZ9:CD9"/>
+    <mergeCell ref="BZ10:CD10"/>
+    <mergeCell ref="BP9:BT9"/>
+    <mergeCell ref="CY9:DC9"/>
+    <mergeCell ref="CJ10:CN10"/>
+    <mergeCell ref="CE10:CI10"/>
+    <mergeCell ref="CO10:CS10"/>
+    <mergeCell ref="CT10:CX10"/>
+    <mergeCell ref="CY10:DC10"/>
+    <mergeCell ref="CE9:CI9"/>
+    <mergeCell ref="CJ9:CN9"/>
+    <mergeCell ref="CO9:CS9"/>
+    <mergeCell ref="CT9:CX9"/>
+    <mergeCell ref="AB9:AF9"/>
+    <mergeCell ref="AG9:AK9"/>
+    <mergeCell ref="AL9:AP9"/>
+    <mergeCell ref="BF9:BJ9"/>
+    <mergeCell ref="BK9:BO9"/>
+    <mergeCell ref="AQ9:AU9"/>
+    <mergeCell ref="AV9:AZ9"/>
+    <mergeCell ref="BA9:BE9"/>
+    <mergeCell ref="FG9:FK9"/>
+    <mergeCell ref="EC9:EG9"/>
+    <mergeCell ref="EH9:EL9"/>
+    <mergeCell ref="EM9:EQ9"/>
+    <mergeCell ref="ER9:EV9"/>
+    <mergeCell ref="EW9:FA9"/>
+    <mergeCell ref="FB9:FF9"/>
+    <mergeCell ref="DD9:DH9"/>
+    <mergeCell ref="DI9:DM9"/>
+    <mergeCell ref="DN9:DR9"/>
+    <mergeCell ref="DS9:DW9"/>
+    <mergeCell ref="DD10:DH10"/>
+    <mergeCell ref="AB10:AF10"/>
+    <mergeCell ref="AG10:AK10"/>
+    <mergeCell ref="AL10:AP10"/>
+    <mergeCell ref="DI10:DM10"/>
+    <mergeCell ref="BF10:BJ10"/>
+    <mergeCell ref="BK10:BO10"/>
+    <mergeCell ref="BP10:BT10"/>
+    <mergeCell ref="BU10:BY10"/>
+    <mergeCell ref="AQ10:AU10"/>
+    <mergeCell ref="AV10:AZ10"/>
+    <mergeCell ref="BA10:BE10"/>
+    <mergeCell ref="FG10:FK10"/>
+    <mergeCell ref="DN10:DR10"/>
+    <mergeCell ref="DS10:DW10"/>
+    <mergeCell ref="DX10:EB10"/>
+    <mergeCell ref="EC10:EG10"/>
+    <mergeCell ref="EH10:EL10"/>
+    <mergeCell ref="EM10:EQ10"/>
+    <mergeCell ref="EW10:FA10"/>
+    <mergeCell ref="FB10:FF10"/>
+    <mergeCell ref="ER10:EV10"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <conditionalFormatting sqref="R135:V149">

</xml_diff>